<commit_message>
Clean up files in home dir (eg pickles) prior to clean push
</commit_message>
<xml_diff>
--- a/assets/1 Month.xlsx
+++ b/assets/1 Month.xlsx
@@ -553,1919 +553,1919 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44402</v>
+        <v>44421</v>
       </c>
       <c r="B2" t="n">
-        <v>0.999843460407399</v>
+        <v>1.003545014639884</v>
       </c>
       <c r="C2" t="n">
-        <v>1.001088099392462</v>
+        <v>1.001755993118152</v>
       </c>
       <c r="D2" t="n">
-        <v>1.000125353137791</v>
+        <v>1.00044819847283</v>
       </c>
       <c r="E2" t="n">
-        <v>1.001191099931314</v>
+        <v>1.001607306655808</v>
       </c>
       <c r="F2" t="n">
-        <v>1.001645061401704</v>
+        <v>0.9906598455934917</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9983946442312612</v>
+        <v>1.002505451896169</v>
       </c>
       <c r="H2" t="n">
-        <v>0.990575473503756</v>
+        <v>0.9971960623744202</v>
       </c>
       <c r="I2" t="n">
-        <v>1.000107445876291</v>
+        <v>1.001145124017773</v>
       </c>
       <c r="J2" t="n">
-        <v>0.99961325023512</v>
+        <v>0.9963804229899763</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9993962341884397</v>
+        <v>1.002343605342839</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9988915336235682</v>
+        <v>0.9906055571189007</v>
       </c>
       <c r="M2" t="n">
-        <v>1.000214137659924</v>
+        <v>1.021860433179279</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9988134969676143</v>
+        <v>1.014325811995228</v>
       </c>
       <c r="O2" t="n">
-        <v>1.00337568426422</v>
+        <v>1.006288632754339</v>
       </c>
       <c r="P2" t="n">
-        <v>1.004926103745908</v>
+        <v>0.9809402671475673</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.043890656318765</v>
+        <v>0.9748571486700148</v>
       </c>
       <c r="R2" t="n">
-        <v>1.005747114932671</v>
+        <v>0.9995268186497722</v>
       </c>
       <c r="S2" t="n">
-        <v>0.9921135646687698</v>
+        <v>0.9896083498143911</v>
       </c>
       <c r="T2" t="n">
-        <v>0.99981123800336</v>
+        <v>1.004699543219765</v>
       </c>
       <c r="U2" t="n">
-        <v>1.007349556456029</v>
+        <v>1.005703855568239</v>
       </c>
       <c r="V2" t="n">
-        <v>1.002699065682293</v>
+        <v>0.9899032219134278</v>
       </c>
       <c r="W2" t="n">
-        <v>0.9976587270306122</v>
+        <v>0.9989335794950475</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44403</v>
+        <v>44423</v>
       </c>
       <c r="B3" t="n">
-        <v>0.9996869208147979</v>
+        <v>0.9990476981774101</v>
       </c>
       <c r="C3" t="n">
-        <v>1.002176198784924</v>
+        <v>1.000159972206782</v>
       </c>
       <c r="D3" t="n">
-        <v>1.000250706275581</v>
+        <v>0.9994647982942092</v>
       </c>
       <c r="E3" t="n">
-        <v>1.002382199862629</v>
+        <v>1.002161008693292</v>
       </c>
       <c r="F3" t="n">
-        <v>1.003290122803408</v>
+        <v>0.9876229246110979</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9967892884625225</v>
+        <v>1.000883179605895</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9811509470075118</v>
+        <v>0.9933406124850954</v>
       </c>
       <c r="I3" t="n">
-        <v>1.000214891752582</v>
+        <v>0.9972413137998802</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9992265004702401</v>
+        <v>0.9939726065555425</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9987924683768794</v>
+        <v>0.9998534984739047</v>
       </c>
       <c r="L3" t="n">
-        <v>0.9977830672471364</v>
+        <v>0.9822950968984896</v>
       </c>
       <c r="M3" t="n">
-        <v>1.000428275319848</v>
+        <v>1.024883713833121</v>
       </c>
       <c r="N3" t="n">
-        <v>0.9976269939352287</v>
+        <v>1.016855688443122</v>
       </c>
       <c r="O3" t="n">
-        <v>1.006751368528439</v>
+        <v>1.004244825110071</v>
       </c>
       <c r="P3" t="n">
-        <v>1.009852207491817</v>
+        <v>0.9917407804109718</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.087781312637531</v>
+        <v>0.9771428426106771</v>
       </c>
       <c r="R3" t="n">
-        <v>1.011494229865343</v>
+        <v>0.9973971415044225</v>
       </c>
       <c r="S3" t="n">
-        <v>0.9842271293375394</v>
+        <v>0.9653277556827555</v>
       </c>
       <c r="T3" t="n">
-        <v>0.9996224760067201</v>
+        <v>1.011916761075838</v>
       </c>
       <c r="U3" t="n">
-        <v>1.014699112912058</v>
+        <v>1.00866984131626</v>
       </c>
       <c r="V3" t="n">
-        <v>1.005398131364586</v>
+        <v>0.9823306918430632</v>
       </c>
       <c r="W3" t="n">
-        <v>0.9952304153322478</v>
+        <v>0.996113514379796</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44404</v>
+        <v>44424</v>
       </c>
       <c r="B4" t="n">
-        <v>0.995517673236628</v>
+        <v>0.9945503817149361</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9997203042154686</v>
+        <v>0.998563951295413</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9881101117232466</v>
+        <v>0.998481398115589</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9976585290701653</v>
+        <v>1.002714710730775</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9919354535757683</v>
+        <v>0.9845860036287041</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9904169138566162</v>
+        <v>0.9992609073156205</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9608401119387916</v>
+        <v>0.9894851625957707</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9919432803791536</v>
+        <v>0.9933375035819875</v>
       </c>
       <c r="J4" t="n">
-        <v>0.9988397507053601</v>
+        <v>0.9915647901211089</v>
       </c>
       <c r="K4" t="n">
-        <v>0.9939622699089771</v>
+        <v>0.9973633916049702</v>
       </c>
       <c r="L4" t="n">
-        <v>0.9941804325952438</v>
+        <v>0.9739846366780786</v>
       </c>
       <c r="M4" t="n">
-        <v>0.9832975892665693</v>
+        <v>1.027906994486964</v>
       </c>
       <c r="N4" t="n">
-        <v>0.9992881162854443</v>
+        <v>1.019385564891017</v>
       </c>
       <c r="O4" t="n">
-        <v>0.9916364951680114</v>
+        <v>1.002201017465803</v>
       </c>
       <c r="P4" t="n">
-        <v>0.9780788207135717</v>
+        <v>1.002541293674376</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.073646997410447</v>
+        <v>0.9794285365513392</v>
       </c>
       <c r="R4" t="n">
-        <v>1.011993991422936</v>
+        <v>0.9952674643590727</v>
       </c>
       <c r="S4" t="n">
-        <v>0.917981072555205</v>
+        <v>0.94104716155112</v>
       </c>
       <c r="T4" t="n">
-        <v>1.002265028755531</v>
+        <v>1.019133978931909</v>
       </c>
       <c r="U4" t="n">
-        <v>1.019751965830687</v>
+        <v>1.01163582706428</v>
       </c>
       <c r="V4" t="n">
-        <v>1.005128271128713</v>
+        <v>0.9747581617726987</v>
       </c>
       <c r="W4" t="n">
-        <v>0.9812485380311514</v>
+        <v>0.9930850221959791</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44405</v>
+        <v>44425</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9984347430350129</v>
+        <v>0.9983178422221399</v>
       </c>
       <c r="C5" t="n">
-        <v>1.005379428200078</v>
+        <v>0.9977554542297721</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9949848213772088</v>
+        <v>0.9891956485201211</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9974727033142949</v>
+        <v>0.9971417875649369</v>
       </c>
       <c r="F5" t="n">
-        <v>1.006928725938671</v>
+        <v>0.9701880313686971</v>
       </c>
       <c r="G5" t="n">
-        <v>0.9936863963042757</v>
+        <v>0.9990237138335086</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9876904143722527</v>
+        <v>0.9712594254128918</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9987109773132661</v>
+        <v>0.9900062553729811</v>
       </c>
       <c r="J5" t="n">
-        <v>1.007488584691959</v>
+        <v>0.9905654514481719</v>
       </c>
       <c r="K5" t="n">
-        <v>1.000301864911925</v>
+        <v>0.9980957944667754</v>
       </c>
       <c r="L5" t="n">
-        <v>1.00443397121994</v>
+        <v>0.9638676122013851</v>
       </c>
       <c r="M5" t="n">
-        <v>0.9922912076130573</v>
+        <v>1.018604633420013</v>
       </c>
       <c r="N5" t="n">
-        <v>1.004330776804178</v>
+        <v>1.017861546296576</v>
       </c>
       <c r="O5" t="n">
-        <v>1.00654979383183</v>
+        <v>0.9749501422564968</v>
       </c>
       <c r="P5" t="n">
-        <v>0.9766009778450414</v>
+        <v>0.9745870632562367</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.056165155887173</v>
+        <v>0.9605714343843005</v>
       </c>
       <c r="R5" t="n">
-        <v>1.011993991422936</v>
+        <v>0.9858022125425554</v>
       </c>
       <c r="S5" t="n">
-        <v>0.9593060129448443</v>
+        <v>0.9116706989836683</v>
       </c>
       <c r="T5" t="n">
-        <v>1.003397485531223</v>
+        <v>1.007385069661316</v>
       </c>
       <c r="U5" t="n">
-        <v>1.014239754681853</v>
+        <v>1.010723189285218</v>
       </c>
       <c r="V5" t="n">
-        <v>1.00863696899902</v>
+        <v>0.9680269407186076</v>
       </c>
       <c r="W5" t="n">
-        <v>0.9996425629695885</v>
+        <v>0.9815887047523306</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44406</v>
+        <v>44426</v>
       </c>
       <c r="B6" t="n">
-        <v>1.007228613464281</v>
+        <v>0.9966773633464874</v>
       </c>
       <c r="C6" t="n">
-        <v>1.007302219360872</v>
+        <v>1.003773123386193</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9960416184264965</v>
+        <v>0.9804033127140065</v>
       </c>
       <c r="E6" t="n">
-        <v>1.001668226097816</v>
+        <v>0.9864240382320939</v>
       </c>
       <c r="F6" t="n">
-        <v>1.013748841805619</v>
+        <v>0.9619931479568927</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9981607135723345</v>
+        <v>1.001785721945023</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9926141734916034</v>
+        <v>0.9718046011731262</v>
       </c>
       <c r="I6" t="n">
-        <v>1.008056719620846</v>
+        <v>0.990318547482697</v>
       </c>
       <c r="J6" t="n">
-        <v>1.011950914373503</v>
+        <v>0.9964512142819751</v>
       </c>
       <c r="K6" t="n">
-        <v>1.00528299583579</v>
+        <v>0.999267597138195</v>
       </c>
       <c r="L6" t="n">
-        <v>1.021477110864398</v>
+        <v>0.9475357023453412</v>
       </c>
       <c r="M6" t="n">
-        <v>1.015845778408569</v>
+        <v>1.012093033901481</v>
       </c>
       <c r="N6" t="n">
-        <v>1.015484104462236</v>
+        <v>1.018654065731674</v>
       </c>
       <c r="O6" t="n">
-        <v>1.002619932908376</v>
+        <v>0.9770464064841456</v>
       </c>
       <c r="P6" t="n">
-        <v>1</v>
+        <v>0.9783989734731909</v>
       </c>
       <c r="Q6" t="n">
-        <v>1.028268559509454</v>
+        <v>0.9487619309198289</v>
       </c>
       <c r="R6" t="n">
-        <v>1.021989031935269</v>
+        <v>0.9858022125425554</v>
       </c>
       <c r="S6" t="n">
-        <v>0.9809148650064078</v>
+        <v>0.935251809968673</v>
       </c>
       <c r="T6" t="n">
-        <v>0.9992450672175881</v>
+        <v>1.008056374439935</v>
       </c>
       <c r="U6" t="n">
-        <v>1.007119833534114</v>
+        <v>1.009354319650555</v>
       </c>
       <c r="V6" t="n">
-        <v>1.026315851792059</v>
+        <v>0.9568083816139611</v>
       </c>
       <c r="W6" t="n">
-        <v>1.003018412555629</v>
+        <v>0.9684522676743533</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44407</v>
+        <v>44427</v>
       </c>
       <c r="B7" t="n">
-        <v>1.000668749924005</v>
+        <v>0.9813295488347082</v>
       </c>
       <c r="C7" t="n">
-        <v>1.002857983931959</v>
+        <v>0.9941086636505806</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9889256146779474</v>
+        <v>0.9814751002679303</v>
       </c>
       <c r="E7" t="n">
-        <v>0.996253159535894</v>
+        <v>0.9876636696592955</v>
       </c>
       <c r="F7" t="n">
-        <v>1.007512546507319</v>
+        <v>0.9502465862993298</v>
       </c>
       <c r="G7" t="n">
-        <v>0.9920289693844691</v>
+        <v>0.9892266610130753</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9829973097199258</v>
+        <v>0.9558376258555926</v>
       </c>
       <c r="I7" t="n">
-        <v>1.000752039176848</v>
+        <v>0.9717884743561478</v>
       </c>
       <c r="J7" t="n">
-        <v>1.015066404092793</v>
+        <v>0.9920447685283241</v>
       </c>
       <c r="K7" t="n">
-        <v>1.000452797367888</v>
+        <v>0.9846198891309978</v>
       </c>
       <c r="L7" t="n">
-        <v>1.026049673417083</v>
+        <v>0.9228211623231642</v>
       </c>
       <c r="M7" t="n">
-        <v>1.011991382215097</v>
+        <v>1.000465126924737</v>
       </c>
       <c r="N7" t="n">
-        <v>1.007475141100349</v>
+        <v>1.015666955799833</v>
       </c>
       <c r="O7" t="n">
-        <v>0.9876058468962531</v>
+        <v>0.9521013819431008</v>
       </c>
       <c r="P7" t="n">
-        <v>0.9642857184802709</v>
+        <v>0.9733163861244383</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.93713964963102</v>
+        <v>0.9519999912806919</v>
       </c>
       <c r="R7" t="n">
-        <v>1.00549728181376</v>
+        <v>0.968291523762198</v>
       </c>
       <c r="S7" t="n">
-        <v>0.979810744806043</v>
+        <v>0.9076738963769644</v>
       </c>
       <c r="T7" t="n">
-        <v>1.002642552748811</v>
+        <v>0.9684458070188791</v>
       </c>
       <c r="U7" t="n">
-        <v>1.007119833534114</v>
+        <v>1.005019333716979</v>
       </c>
       <c r="V7" t="n">
-        <v>1.030094512859031</v>
+        <v>0.9318468549047669</v>
       </c>
       <c r="W7" t="n">
-        <v>0.995052978461677</v>
+        <v>0.9673824712699151</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44409</v>
+        <v>44428</v>
       </c>
       <c r="B8" t="n">
-        <v>1.004183491083044</v>
+        <v>0.9853611341114392</v>
       </c>
       <c r="C8" t="n">
-        <v>1.008536738685699</v>
+        <v>1.000172638386651</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9892083750244683</v>
+        <v>0.993142695188787</v>
       </c>
       <c r="E8" t="n">
-        <v>0.995335209077771</v>
+        <v>0.9957048002469411</v>
       </c>
       <c r="F8" t="n">
-        <v>1.005080034463534</v>
+        <v>0.9659235369780445</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9928056740166451</v>
+        <v>0.9918764142914127</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9865748018259268</v>
+        <v>0.9547472743351236</v>
       </c>
       <c r="I8" t="n">
-        <v>1.002685614185544</v>
+        <v>0.9758484306288985</v>
       </c>
       <c r="J8" t="n">
-        <v>1.017703235268251</v>
+        <v>0.9923752879798404</v>
       </c>
       <c r="K8" t="n">
-        <v>1.003849029541016</v>
+        <v>0.9882818335942424</v>
       </c>
       <c r="L8" t="n">
-        <v>1.007413103445797</v>
+        <v>0.9228211623231642</v>
       </c>
       <c r="M8" t="n">
-        <v>1.00985008730102</v>
+        <v>0.9930232735567316</v>
       </c>
       <c r="N8" t="n">
-        <v>1.006852197587923</v>
+        <v>1.01621558016934</v>
       </c>
       <c r="O8" t="n">
-        <v>0.9897723136154789</v>
+        <v>0.9733780440411401</v>
       </c>
       <c r="P8" t="n">
-        <v>0.9667487703532249</v>
+        <v>0.9783989734731908</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.9197507811545017</v>
+        <v>0.9443809872581844</v>
       </c>
       <c r="R8" t="n">
-        <v>1.017741154015493</v>
+        <v>0.9446284844882361</v>
       </c>
       <c r="S8" t="n">
-        <v>0.9911671828020258</v>
+        <v>0.9486411230956776</v>
       </c>
       <c r="T8" t="n">
-        <v>1.029256381416972</v>
+        <v>0.9835515475096416</v>
       </c>
       <c r="U8" t="n">
-        <v>1.006430839995619</v>
+        <v>1.011179508174749</v>
       </c>
       <c r="V8" t="n">
-        <v>1.006882620063867</v>
+        <v>0.9140373374942119</v>
       </c>
       <c r="W8" t="n">
-        <v>0.9914498418994718</v>
+        <v>0.9838310012276351</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44410</v>
+        <v>44430</v>
       </c>
       <c r="B9" t="n">
-        <v>1.007698232242084</v>
+        <v>0.9868278038191723</v>
       </c>
       <c r="C9" t="n">
-        <v>1.01421549343944</v>
+        <v>0.9999536532963899</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9894911353709893</v>
+        <v>1.000836615178768</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9944172586196479</v>
+        <v>0.9999483897379315</v>
       </c>
       <c r="F9" t="n">
-        <v>1.002647522419748</v>
+        <v>0.9749918703927918</v>
       </c>
       <c r="G9" t="n">
-        <v>0.9935823786488213</v>
+        <v>0.9932803349997946</v>
       </c>
       <c r="H9" t="n">
-        <v>0.9901522939319278</v>
+        <v>0.9619908194835965</v>
       </c>
       <c r="I9" t="n">
-        <v>1.004619189194239</v>
+        <v>0.9808453029424079</v>
       </c>
       <c r="J9" t="n">
-        <v>1.020340066443709</v>
+        <v>0.9942637441485525</v>
       </c>
       <c r="K9" t="n">
-        <v>1.007245261714143</v>
+        <v>0.9915043084020914</v>
       </c>
       <c r="L9" t="n">
-        <v>0.9887765334745113</v>
+        <v>0.9472466917605629</v>
       </c>
       <c r="M9" t="n">
-        <v>1.007708792386943</v>
+        <v>1.005348826563636</v>
       </c>
       <c r="N9" t="n">
-        <v>1.006229254075498</v>
+        <v>1.022403091942021</v>
       </c>
       <c r="O9" t="n">
-        <v>0.9919387803347047</v>
+        <v>0.9826537833511122</v>
       </c>
       <c r="P9" t="n">
-        <v>0.9692118222261791</v>
+        <v>0.9904701335737834</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.9023619126779834</v>
+        <v>0.947904786609468</v>
       </c>
       <c r="R9" t="n">
-        <v>1.029985026217226</v>
+        <v>0.9446284844882361</v>
       </c>
       <c r="S9" t="n">
-        <v>1.002523620798009</v>
+        <v>0.9727218344065205</v>
       </c>
       <c r="T9" t="n">
-        <v>1.055870210085132</v>
+        <v>0.9897617057554268</v>
       </c>
       <c r="U9" t="n">
-        <v>1.005741846457124</v>
+        <v>1.020077508935774</v>
       </c>
       <c r="V9" t="n">
-        <v>0.9836707272687025</v>
+        <v>0.9390688885883682</v>
       </c>
       <c r="W9" t="n">
-        <v>0.9877249853698636</v>
+        <v>0.9960218354570692</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44411</v>
+        <v>44431</v>
       </c>
       <c r="B10" t="n">
-        <v>1.01111333834751</v>
+        <v>0.9882944735269055</v>
       </c>
       <c r="C10" t="n">
-        <v>1.017755177167265</v>
+        <v>0.9997346682061286</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9948978738870424</v>
+        <v>1.00853053516875</v>
       </c>
       <c r="E10" t="n">
-        <v>1.002574887558263</v>
+        <v>1.004191979228922</v>
       </c>
       <c r="F10" t="n">
-        <v>1.00630424564836</v>
+        <v>0.9840602038075391</v>
       </c>
       <c r="G10" t="n">
-        <v>0.9927112229939722</v>
+        <v>0.9946842557081765</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9946145562878603</v>
+        <v>0.9692343646320694</v>
       </c>
       <c r="I10" t="n">
-        <v>1.006015739714454</v>
+        <v>0.9858421752559174</v>
       </c>
       <c r="J10" t="n">
-        <v>1.021216270072362</v>
+        <v>0.9961522003172643</v>
       </c>
       <c r="K10" t="n">
-        <v>1.009660396935805</v>
+        <v>0.9947267832099403</v>
       </c>
       <c r="L10" t="n">
-        <v>0.9790772544665842</v>
+        <v>0.9716722211979615</v>
       </c>
       <c r="M10" t="n">
-        <v>1.01413275881434</v>
+        <v>1.01767437957054</v>
       </c>
       <c r="N10" t="n">
-        <v>1.005517370360942</v>
+        <v>1.028590603714702</v>
       </c>
       <c r="O10" t="n">
-        <v>0.9876058468962533</v>
+        <v>0.9919295226610843</v>
       </c>
       <c r="P10" t="n">
-        <v>0.9913793478065552</v>
+        <v>1.002541293674376</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.9179840094872946</v>
+        <v>0.9514285859607515</v>
       </c>
       <c r="R10" t="n">
-        <v>1.023488221288279</v>
+        <v>0.9446284844882361</v>
       </c>
       <c r="S10" t="n">
-        <v>0.9566246056782334</v>
+        <v>0.9968025457173633</v>
       </c>
       <c r="T10" t="n">
-        <v>1.057757714847384</v>
+        <v>0.995971864001212</v>
       </c>
       <c r="U10" t="n">
-        <v>1.014010119373562</v>
+        <v>1.028975509696798</v>
       </c>
       <c r="V10" t="n">
-        <v>0.9771930519998333</v>
+        <v>0.9641004396825246</v>
       </c>
       <c r="W10" t="n">
-        <v>1.006154435994407</v>
+        <v>1.008096605955071</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44412</v>
+        <v>44432</v>
       </c>
       <c r="B11" t="n">
-        <v>1.013703085455818</v>
+        <v>0.990629985431391</v>
       </c>
       <c r="C11" t="n">
-        <v>1.020289765515584</v>
+        <v>1.0058618093457</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9961946486419669</v>
+        <v>1.013737612749928</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9979305717788782</v>
+        <v>1.005693985625749</v>
       </c>
       <c r="F11" t="n">
-        <v>0.993967445263507</v>
+        <v>0.9941355858555605</v>
       </c>
       <c r="G11" t="n">
-        <v>1.001457618289856</v>
+        <v>0.9980134816093862</v>
       </c>
       <c r="H11" t="n">
-        <v>0.9999229899580782</v>
+        <v>0.9917439244611158</v>
       </c>
       <c r="I11" t="n">
-        <v>1.011816587676327</v>
+        <v>0.9870914231180031</v>
       </c>
       <c r="J11" t="n">
-        <v>1.021370474780152</v>
+        <v>1.001196055858844</v>
       </c>
       <c r="K11" t="n">
-        <v>1.01584905948279</v>
+        <v>0.9947267832099403</v>
       </c>
       <c r="L11" t="n">
-        <v>0.9456838261271833</v>
+        <v>0.9991327477110714</v>
       </c>
       <c r="M11" t="n">
-        <v>1.008137067706791</v>
+        <v>1.026976740637491</v>
       </c>
       <c r="N11" t="n">
-        <v>1.005754634757668</v>
+        <v>1.028102906602236</v>
       </c>
       <c r="O11" t="n">
-        <v>0.9627166764622335</v>
+        <v>0.9888899995042214</v>
       </c>
       <c r="P11" t="n">
-        <v>1.024630518729542</v>
+        <v>0.9898348253024944</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.9103589426485066</v>
+        <v>0.9832380748930433</v>
       </c>
       <c r="R11" t="n">
-        <v>1.015492227006322</v>
+        <v>0.9592996338305709</v>
       </c>
       <c r="S11" t="n">
-        <v>0.8903785488958991</v>
+        <v>0.9594324779365041</v>
       </c>
       <c r="T11" t="n">
-        <v>1.065307733896389</v>
+        <v>1.000335703610489</v>
       </c>
       <c r="U11" t="n">
-        <v>1.010335341145548</v>
+        <v>1.033310495630375</v>
       </c>
       <c r="V11" t="n">
-        <v>0.9497975533426994</v>
+        <v>0.9963540244602824</v>
       </c>
       <c r="W11" t="n">
-        <v>1.023363409088055</v>
+        <v>1.014409786899315</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44413</v>
+        <v>44433</v>
       </c>
       <c r="B12" t="n">
-        <v>1.013205049148777</v>
+        <v>0.9940082165814965</v>
       </c>
       <c r="C12" t="n">
-        <v>1.027211830764676</v>
+        <v>1.010089763736267</v>
       </c>
       <c r="D12" t="n">
-        <v>1.003917902613282</v>
+        <v>1.015226554441284</v>
       </c>
       <c r="E12" t="n">
-        <v>1.003923590751256</v>
+        <v>1.007926745171184</v>
       </c>
       <c r="F12" t="n">
-        <v>1.011929540237988</v>
+        <v>0.9978610075969534</v>
       </c>
       <c r="G12" t="n">
-        <v>1.004810676337255</v>
+        <v>0.9951780666801061</v>
       </c>
       <c r="H12" t="n">
-        <v>0.9979227010765062</v>
+        <v>0.9931458457350357</v>
       </c>
       <c r="I12" t="n">
-        <v>1.015576373774617</v>
+        <v>0.9889652551995206</v>
       </c>
       <c r="J12" t="n">
-        <v>1.019114946189787</v>
+        <v>1.007026780144051</v>
       </c>
       <c r="K12" t="n">
-        <v>1.019471726327572</v>
+        <v>0.9945803166067356</v>
       </c>
       <c r="L12" t="n">
-        <v>0.9587086628357249</v>
+        <v>1.010984166498325</v>
       </c>
       <c r="M12" t="n">
-        <v>0.9978586234007577</v>
+        <v>1.027441867562228</v>
       </c>
       <c r="N12" t="n">
-        <v>1.001779799810768</v>
+        <v>1.020970510742499</v>
       </c>
       <c r="O12" t="n">
-        <v>0.9475010157535009</v>
+        <v>0.9768367400792287</v>
       </c>
       <c r="P12" t="n">
-        <v>1.019704414983633</v>
+        <v>0.9898348253024944</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.9205876804647275</v>
+        <v>0.9801523844401043</v>
       </c>
       <c r="R12" t="n">
-        <v>1.023488221288279</v>
+        <v>0.9753905077582515</v>
       </c>
       <c r="S12" t="n">
-        <v>0.8247634454480481</v>
+        <v>0.9814148922733745</v>
       </c>
       <c r="T12" t="n">
-        <v>1.069082743420892</v>
+        <v>0.9996642963895109</v>
       </c>
       <c r="U12" t="n">
-        <v>1.016536458219253</v>
+        <v>1.028975509696798</v>
       </c>
       <c r="V12" t="n">
-        <v>0.9620783047711516</v>
+        <v>1.013181916611817</v>
       </c>
       <c r="W12" t="n">
-        <v>1.035992016844172</v>
+        <v>1.019752980168539</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44414</v>
+        <v>44434</v>
       </c>
       <c r="B13" t="n">
-        <v>1.013575032872967</v>
+        <v>0.9905187964382053</v>
       </c>
       <c r="C13" t="n">
-        <v>1.025031193718905</v>
+        <v>1.008657991923583</v>
       </c>
       <c r="D13" t="n">
-        <v>0.999917067496132</v>
+        <v>1.008743759001044</v>
       </c>
       <c r="E13" t="n">
-        <v>1.005605430052153</v>
+        <v>1.002055653704446</v>
       </c>
       <c r="F13" t="n">
-        <v>1.017247124705797</v>
+        <v>0.9865912886077467</v>
       </c>
       <c r="G13" t="n">
-        <v>1.005881578298714</v>
+        <v>0.9909716354340469</v>
       </c>
       <c r="H13" t="n">
-        <v>0.9893060287029571</v>
+        <v>0.9827868407464018</v>
       </c>
       <c r="I13" t="n">
-        <v>1.0177247995573</v>
+        <v>0.9863627150542587</v>
       </c>
       <c r="J13" t="n">
-        <v>1.023601639620924</v>
+        <v>1.006814310214742</v>
       </c>
       <c r="K13" t="n">
-        <v>1.019320721896189</v>
+        <v>0.9915043084020914</v>
       </c>
       <c r="L13" t="n">
-        <v>0.9474850905960234</v>
+        <v>0.9973984636678078</v>
       </c>
       <c r="M13" t="n">
-        <v>0.9644539653042262</v>
+        <v>1.01627908751022</v>
       </c>
       <c r="N13" t="n">
-        <v>0.9767441965726021</v>
+        <v>1.022128779757268</v>
       </c>
       <c r="O13" t="n">
-        <v>0.9225111348493976</v>
+        <v>0.9568179164820825</v>
       </c>
       <c r="P13" t="n">
-        <v>1.019704414983633</v>
+        <v>1.063278291257957</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.9217035698599331</v>
+        <v>0.981714303152902</v>
       </c>
       <c r="R13" t="n">
-        <v>1.035482212711215</v>
+        <v>0.969711338614875</v>
       </c>
       <c r="S13" t="n">
-        <v>0.8700315072333399</v>
+        <v>0.9894084974867821</v>
       </c>
       <c r="T13" t="n">
-        <v>1.085315238294596</v>
+        <v>1.000335703610488</v>
       </c>
       <c r="U13" t="n">
-        <v>1.002526426459314</v>
+        <v>1.014829972257065</v>
       </c>
       <c r="V13" t="n">
-        <v>0.9541160378422096</v>
+        <v>0.9966344429675189</v>
       </c>
       <c r="W13" t="n">
-        <v>1.020667134972022</v>
+        <v>1.013071661173924</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44416</v>
+        <v>44435</v>
       </c>
       <c r="B14" t="n">
-        <v>1.014236695784791</v>
+        <v>0.9937162606231987</v>
       </c>
       <c r="C14" t="n">
-        <v>1.024970039605503</v>
+        <v>1.013176445971917</v>
       </c>
       <c r="D14" t="n">
-        <v>1.000740008048402</v>
+        <v>1.021141653786453</v>
       </c>
       <c r="E14" t="n">
-        <v>1.005132841620011</v>
+        <v>1.010881391627207</v>
       </c>
       <c r="F14" t="n">
-        <v>1.014316807292586</v>
+        <v>1.014740998710686</v>
       </c>
       <c r="G14" t="n">
-        <v>1.00536974786407</v>
+        <v>0.9946189983952216</v>
       </c>
       <c r="H14" t="n">
-        <v>0.9910755222454773</v>
+        <v>0.9953267389314533</v>
       </c>
       <c r="I14" t="n">
-        <v>1.018476756776958</v>
+        <v>0.9912555032350666</v>
       </c>
       <c r="J14" t="n">
-        <v>1.024615805457639</v>
+        <v>1.008159825029284</v>
       </c>
       <c r="K14" t="n">
-        <v>1.020150922379404</v>
+        <v>0.99589858588136</v>
       </c>
       <c r="L14" t="n">
-        <v>0.9350145663613573</v>
+        <v>1.016476360014785</v>
       </c>
       <c r="M14" t="n">
-        <v>0.9479657330733022</v>
+        <v>1.038604647614235</v>
       </c>
       <c r="N14" t="n">
-        <v>0.9680825977020567</v>
+        <v>1.03749091323447</v>
       </c>
       <c r="O14" t="n">
-        <v>0.9217553834935541</v>
+        <v>0.9885755798611501</v>
       </c>
       <c r="P14" t="n">
-        <v>1.009852207491817</v>
+        <v>1.115628953067953</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.9275618295591572</v>
+        <v>1.004571460542225</v>
       </c>
       <c r="R14" t="n">
-        <v>1.03473261803471</v>
+        <v>0.9734974212880156</v>
       </c>
       <c r="S14" t="n">
-        <v>0.8530756712711948</v>
+        <v>0.9696243367808722</v>
       </c>
       <c r="T14" t="n">
-        <v>1.088901485822459</v>
+        <v>0.9993286952213811</v>
       </c>
       <c r="U14" t="n">
-        <v>1.004019274997262</v>
+        <v>1.014601856329264</v>
       </c>
       <c r="V14" t="n">
-        <v>0.9429149847592289</v>
+        <v>1.01949234942136</v>
       </c>
       <c r="W14" t="n">
-        <v>1.025731976160982</v>
+        <v>1.02749000028674</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44417</v>
+        <v>44437</v>
       </c>
       <c r="B15" t="n">
-        <v>1.014898358696615</v>
+        <v>0.9924048459575379</v>
       </c>
       <c r="C15" t="n">
-        <v>1.024908885492102</v>
+        <v>1.013773017560535</v>
       </c>
       <c r="D15" t="n">
-        <v>1.001562948600672</v>
+        <v>1.025744355500483</v>
       </c>
       <c r="E15" t="n">
-        <v>1.004660253187869</v>
+        <v>1.013058107791563</v>
       </c>
       <c r="F15" t="n">
-        <v>1.011386489879375</v>
+        <v>1.012254464919535</v>
       </c>
       <c r="G15" t="n">
-        <v>1.004857917429426</v>
+        <v>0.9957345920743921</v>
       </c>
       <c r="H15" t="n">
-        <v>0.9928450157879976</v>
+        <v>0.9962224187796027</v>
       </c>
       <c r="I15" t="n">
-        <v>1.019228713996616</v>
+        <v>0.991984211298811</v>
       </c>
       <c r="J15" t="n">
-        <v>1.025629971294353</v>
+        <v>1.011244353065726</v>
       </c>
       <c r="K15" t="n">
-        <v>1.020981122862618</v>
+        <v>0.99589858588136</v>
       </c>
       <c r="L15" t="n">
-        <v>0.9225440421266912</v>
+        <v>1.019872813289238</v>
       </c>
       <c r="M15" t="n">
-        <v>0.9314775008423782</v>
+        <v>1.036976747734602</v>
       </c>
       <c r="N15" t="n">
-        <v>0.9594209988315112</v>
+        <v>1.034930573158055</v>
       </c>
       <c r="O15" t="n">
-        <v>0.9209996321377105</v>
+        <v>0.9878943239737783</v>
       </c>
       <c r="P15" t="n">
-        <v>1</v>
+        <v>1.104828439804548</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.9334200892583815</v>
+        <v>1.024095262799944</v>
       </c>
       <c r="R15" t="n">
-        <v>1.033983023358205</v>
+        <v>0.9673450256607456</v>
       </c>
       <c r="S15" t="n">
-        <v>0.8361198353090497</v>
+        <v>0.9679256834757496</v>
       </c>
       <c r="T15" t="n">
-        <v>1.092487733350322</v>
+        <v>1.000335703610488</v>
       </c>
       <c r="U15" t="n">
-        <v>1.00551212353521</v>
+        <v>1.008898000761025</v>
       </c>
       <c r="V15" t="n">
-        <v>0.9317139316762481</v>
+        <v>1.024470660585119</v>
       </c>
       <c r="W15" t="n">
-        <v>1.030567611485459</v>
+        <v>1.030935578901838</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44418</v>
+        <v>44438</v>
       </c>
       <c r="B16" t="n">
-        <v>1.018982284206558</v>
+        <v>0.9910934312918771</v>
       </c>
       <c r="C16" t="n">
-        <v>1.030096017505866</v>
+        <v>1.014369589149153</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9967041569851743</v>
+        <v>1.030347057214512</v>
       </c>
       <c r="E16" t="n">
-        <v>1.005657558659071</v>
+        <v>1.015234823955919</v>
       </c>
       <c r="F16" t="n">
-        <v>1.013445661707138</v>
+        <v>1.009767931128383</v>
       </c>
       <c r="G16" t="n">
-        <v>1.006472528214244</v>
+        <v>0.9968501857535627</v>
       </c>
       <c r="H16" t="n">
-        <v>0.9946145562878603</v>
+        <v>0.9971180986277522</v>
       </c>
       <c r="I16" t="n">
-        <v>1.020088117092565</v>
+        <v>0.9927129193625555</v>
       </c>
       <c r="J16" t="n">
-        <v>1.026644137131068</v>
+        <v>1.014328881102167</v>
       </c>
       <c r="K16" t="n">
-        <v>1.024452857251437</v>
+        <v>0.99589858588136</v>
       </c>
       <c r="L16" t="n">
-        <v>0.9476236819287687</v>
+        <v>1.023269266563692</v>
       </c>
       <c r="M16" t="n">
-        <v>0.925910085054678</v>
+        <v>1.035348847854969</v>
       </c>
       <c r="N16" t="n">
-        <v>0.9597176472207023</v>
+        <v>1.03237023308164</v>
       </c>
       <c r="O16" t="n">
-        <v>0.9365175780131363</v>
+        <v>0.9872130680864065</v>
       </c>
       <c r="P16" t="n">
-        <v>1.007389214342651</v>
+        <v>1.094027926541144</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.944764716469808</v>
+        <v>1.043619065057664</v>
       </c>
       <c r="R16" t="n">
-        <v>1.029985026217226</v>
+        <v>0.9611926300334757</v>
       </c>
       <c r="S16" t="n">
-        <v>0.7966877067878795</v>
+        <v>0.9662270301706269</v>
       </c>
       <c r="T16" t="n">
-        <v>1.103057829141419</v>
+        <v>1.001342711999596</v>
       </c>
       <c r="U16" t="n">
-        <v>1.013550761143358</v>
+        <v>1.003194145192786</v>
       </c>
       <c r="V16" t="n">
-        <v>0.9531713725754665</v>
+        <v>1.029448971748878</v>
       </c>
       <c r="W16" t="n">
-        <v>1.011760344805696</v>
+        <v>1.034342683665026</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44419</v>
+        <v>44439</v>
       </c>
       <c r="B17" t="n">
-        <v>1.027391996887273</v>
+        <v>0.9897820166262162</v>
       </c>
       <c r="C17" t="n">
-        <v>1.038167421611992</v>
+        <v>1.014966160737771</v>
       </c>
       <c r="D17" t="n">
-        <v>0.9951573341491433</v>
+        <v>1.029898265537822</v>
       </c>
       <c r="E17" t="n">
-        <v>1.006940520042066</v>
+        <v>1.013865154371056</v>
       </c>
       <c r="F17" t="n">
-        <v>1.013160491213633</v>
+        <v>1.013234859102946</v>
       </c>
       <c r="G17" t="n">
-        <v>1.010006822536095</v>
+        <v>0.9935736558984952</v>
       </c>
       <c r="H17" t="n">
-        <v>0.9969995197202993</v>
+        <v>1.011916758678149</v>
       </c>
       <c r="I17" t="n">
-        <v>1.023847903190856</v>
+        <v>0.9902145030616063</v>
       </c>
       <c r="J17" t="n">
-        <v>1.028786067262965</v>
+        <v>1.017413409138608</v>
       </c>
       <c r="K17" t="n">
-        <v>1.028981118831994</v>
+        <v>0.9932620473321114</v>
       </c>
       <c r="L17" t="n">
-        <v>0.9609255955885885</v>
+        <v>1.013007571393664</v>
       </c>
       <c r="M17" t="n">
-        <v>0.9353318970358495</v>
+        <v>1.02976741347202</v>
       </c>
       <c r="N17" t="n">
-        <v>0.9729473325543407</v>
+        <v>1.034442876045588</v>
       </c>
       <c r="O17" t="n">
-        <v>0.9628174638105383</v>
+        <v>0.9932920344358283</v>
       </c>
       <c r="P17" t="n">
-        <v>1</v>
+        <v>1.111817042850999</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.9691277695131127</v>
+        <v>1.023999968029204</v>
       </c>
       <c r="R17" t="n">
-        <v>1.036481735826403</v>
+        <v>0.9465215709584721</v>
       </c>
       <c r="S17" t="n">
-        <v>0.7790220723919311</v>
+        <v>0.9648281248637335</v>
       </c>
       <c r="T17" t="n">
-        <v>1.118157867239431</v>
+        <v>1.03793225425333</v>
       </c>
       <c r="U17" t="n">
-        <v>1.007349556456029</v>
+        <v>0.9974902896245463</v>
       </c>
       <c r="V17" t="n">
-        <v>0.9641026169029704</v>
+        <v>1.023559113205625</v>
       </c>
       <c r="W17" t="n">
-        <v>1.00698045893396</v>
+        <v>1.028126640332833</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>44420</v>
+        <v>44440</v>
       </c>
       <c r="B18" t="n">
-        <v>1.023564246023543</v>
+        <v>0.9939664697983405</v>
       </c>
       <c r="C18" t="n">
-        <v>1.037730423620902</v>
+        <v>1.021223911576247</v>
       </c>
       <c r="D18" t="n">
-        <v>0.9986027847681685</v>
+        <v>1.033282361742306</v>
       </c>
       <c r="E18" t="n">
-        <v>1.011115678359191</v>
+        <v>1.014181164607729</v>
       </c>
       <c r="F18" t="n">
-        <v>1.015577203419924</v>
+        <v>1.019157151481373</v>
       </c>
       <c r="G18" t="n">
-        <v>1.01711754175804</v>
+        <v>0.9928960215097908</v>
       </c>
       <c r="H18" t="n">
-        <v>0.9877673304994888</v>
+        <v>1.025001927701175</v>
       </c>
       <c r="I18" t="n">
-        <v>1.031904622811702</v>
+        <v>0.999479539624881</v>
       </c>
       <c r="J18" t="n">
-        <v>1.031090224312883</v>
+        <v>1.026367979283222</v>
       </c>
       <c r="K18" t="n">
-        <v>1.03049058734246</v>
+        <v>0.9975098582081753</v>
       </c>
       <c r="L18" t="n">
-        <v>0.9587086628357249</v>
+        <v>1.014308394693408</v>
       </c>
       <c r="M18" t="n">
-        <v>0.9207708629016612</v>
+        <v>1.040465155313181</v>
       </c>
       <c r="N18" t="n">
-        <v>0.9731845969510663</v>
+        <v>1.034503803302629</v>
       </c>
       <c r="O18" t="n">
-        <v>0.9614067484471561</v>
+        <v>0.9802955160816216</v>
       </c>
       <c r="P18" t="n">
-        <v>0.9692118222261791</v>
+        <v>1.172808091036031</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.9763808732201655</v>
+        <v>1.026857139950707</v>
       </c>
       <c r="R18" t="n">
-        <v>1.055971959973703</v>
+        <v>0.9327969648512553</v>
       </c>
       <c r="S18" t="n">
-        <v>0.7892744383225305</v>
+        <v>0.9542366223505158</v>
       </c>
       <c r="T18" t="n">
-        <v>1.124575314308597</v>
+        <v>1.06008725835256</v>
       </c>
       <c r="U18" t="n">
-        <v>1.006660562917534</v>
+        <v>0.9995436811104698</v>
       </c>
       <c r="V18" t="n">
-        <v>0.9623481650070246</v>
+        <v>1.003926501036082</v>
       </c>
       <c r="W18" t="n">
-        <v>1.016144802518689</v>
+        <v>1.035090135544384</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>44421</v>
+        <v>44441</v>
       </c>
       <c r="B19" t="n">
-        <v>1.027192796260559</v>
+        <v>0.995926667940113</v>
       </c>
       <c r="C19" t="n">
-        <v>1.039552671103277</v>
+        <v>1.020192193652402</v>
       </c>
       <c r="D19" t="n">
-        <v>0.999050357011265</v>
+        <v>1.034753705052449</v>
       </c>
       <c r="E19" t="n">
-        <v>1.01274085131881</v>
+        <v>1.017064114941472</v>
       </c>
       <c r="F19" t="n">
-        <v>1.006091555528253</v>
+        <v>1.026714830350954</v>
       </c>
       <c r="G19" t="n">
-        <v>1.019665880831665</v>
+        <v>0.9939187537262538</v>
       </c>
       <c r="H19" t="n">
-        <v>0.9849976925161827</v>
+        <v>1.019705527125726</v>
       </c>
       <c r="I19" t="n">
-        <v>1.033086281579335</v>
+        <v>1.001769787660427</v>
       </c>
       <c r="J19" t="n">
-        <v>1.0273581138417</v>
+        <v>1.028964684558518</v>
       </c>
       <c r="K19" t="n">
-        <v>1.032905650588702</v>
+        <v>1.00087886946501</v>
       </c>
       <c r="L19" t="n">
-        <v>0.9497021290630996</v>
+        <v>1.034542553914092</v>
       </c>
       <c r="M19" t="n">
-        <v>0.9408993128235498</v>
+        <v>1.02976741347202</v>
       </c>
       <c r="N19" t="n">
-        <v>0.9871262565236391</v>
+        <v>1.031760588436379</v>
       </c>
       <c r="O19" t="n">
-        <v>0.9674526824156831</v>
+        <v>0.9785137514613481</v>
       </c>
       <c r="P19" t="n">
-        <v>0.9507389038171287</v>
+        <v>1.179161355516582</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.9518318740833498</v>
+        <v>1.013904753185454</v>
       </c>
       <c r="R19" t="n">
-        <v>1.05547229373588</v>
+        <v>0.9323237835010276</v>
       </c>
       <c r="S19" t="n">
-        <v>0.7810725744590398</v>
+        <v>1.032973682491674</v>
       </c>
       <c r="T19" t="n">
-        <v>1.129860304602071</v>
+        <v>1.088620323724</v>
       </c>
       <c r="U19" t="n">
-        <v>1.012402409374658</v>
+        <v>0.9977184055523474</v>
       </c>
       <c r="V19" t="n">
-        <v>0.9526315491429287</v>
+        <v>1.024120057209227</v>
       </c>
       <c r="W19" t="n">
-        <v>1.014809529208791</v>
+        <v>1.040214500193117</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>44423</v>
+        <v>44442</v>
       </c>
       <c r="B20" t="n">
-        <v>1.022589503926517</v>
+        <v>0.9923816533002289</v>
       </c>
       <c r="C20" t="n">
-        <v>1.037896431646814</v>
+        <v>1.018857227643001</v>
       </c>
       <c r="D20" t="n">
-        <v>0.9980683308543532</v>
+        <v>1.036936431615129</v>
       </c>
       <c r="E20" t="n">
-        <v>1.014067972604481</v>
+        <v>1.016723366806119</v>
       </c>
       <c r="F20" t="n">
-        <v>1.003007327809946</v>
+        <v>1.021380785361942</v>
       </c>
       <c r="G20" t="n">
-        <v>1.018015839227719</v>
+        <v>0.990192346695866</v>
       </c>
       <c r="H20" t="n">
-        <v>0.9811894050711298</v>
+        <v>1.025391366123554</v>
       </c>
       <c r="I20" t="n">
-        <v>1.029057921768912</v>
+        <v>0.993753919536016</v>
       </c>
       <c r="J20" t="n">
-        <v>1.024875437854216</v>
+        <v>1.030916103674184</v>
       </c>
       <c r="K20" t="n">
-        <v>1.030339618898788</v>
+        <v>0.9956056526749507</v>
       </c>
       <c r="L20" t="n">
-        <v>0.9417348188576398</v>
+        <v>1.024425419170101</v>
       </c>
       <c r="M20" t="n">
-        <v>0.9436830615599825</v>
+        <v>1.064186007477516</v>
       </c>
       <c r="N20" t="n">
-        <v>0.989588293314919</v>
+        <v>1.042794468177136</v>
       </c>
       <c r="O20" t="n">
-        <v>0.9654877519539563</v>
+        <v>1.001467344977203</v>
       </c>
       <c r="P20" t="n">
-        <v>0.9612068889581309</v>
+        <v>1.196950471826436</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.9540635819290477</v>
+        <v>1.01942858014788</v>
       </c>
       <c r="R20" t="n">
-        <v>1.053223414386594</v>
+        <v>0.9313772402659096</v>
       </c>
       <c r="S20" t="n">
-        <v>0.7619085221636558</v>
+        <v>1.093525217588688</v>
       </c>
       <c r="T20" t="n">
-        <v>1.137976609640997</v>
+        <v>1.109432718265994</v>
       </c>
       <c r="U20" t="n">
-        <v>1.015388150257365</v>
+        <v>0.979922404030298</v>
       </c>
       <c r="V20" t="n">
-        <v>0.9453441387252528</v>
+        <v>1.018230305655103</v>
       </c>
       <c r="W20" t="n">
-        <v>1.011816997543355</v>
+        <v>1.043203625134806</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>44424</v>
+        <v>44444</v>
       </c>
       <c r="B21" t="n">
-        <v>1.017986211592476</v>
+        <v>0.9957737661042456</v>
       </c>
       <c r="C21" t="n">
-        <v>1.036240192190351</v>
+        <v>1.019990028262031</v>
       </c>
       <c r="D21" t="n">
-        <v>0.9970863046974415</v>
+        <v>1.03717964519818</v>
       </c>
       <c r="E21" t="n">
-        <v>1.015395093890151</v>
+        <v>1.015572580192022</v>
       </c>
       <c r="F21" t="n">
-        <v>0.999923100091639</v>
+        <v>1.018938802579846</v>
       </c>
       <c r="G21" t="n">
-        <v>1.016365797623773</v>
+        <v>0.9949270864417363</v>
       </c>
       <c r="H21" t="n">
-        <v>0.977381117626077</v>
+        <v>1.027624140073343</v>
       </c>
       <c r="I21" t="n">
-        <v>1.025029561958488</v>
+        <v>0.9995315618354264</v>
       </c>
       <c r="J21" t="n">
-        <v>1.022392761866731</v>
+        <v>1.032454445515439</v>
       </c>
       <c r="K21" t="n">
-        <v>1.027773587208874</v>
+        <v>0.9991210956120998</v>
       </c>
       <c r="L21" t="n">
-        <v>0.9337675086521799</v>
+        <v>1.019896851559929</v>
       </c>
       <c r="M21" t="n">
-        <v>0.9464668102964151</v>
+        <v>1.058449589928915</v>
       </c>
       <c r="N21" t="n">
-        <v>0.9920503301061991</v>
+        <v>1.03598720372571</v>
       </c>
       <c r="O21" t="n">
-        <v>0.9635228214922296</v>
+        <v>0.992907779300654</v>
       </c>
       <c r="P21" t="n">
-        <v>0.9716748740991331</v>
+        <v>1.185091101346013</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.9562952897747454</v>
+        <v>1.018349202473958</v>
       </c>
       <c r="R21" t="n">
-        <v>1.050974535037308</v>
+        <v>0.9253825867999375</v>
       </c>
       <c r="S21" t="n">
-        <v>0.7427444698682718</v>
+        <v>1.07407410343788</v>
       </c>
       <c r="T21" t="n">
-        <v>1.146092914679922</v>
+        <v>1.117377225649886</v>
       </c>
       <c r="U21" t="n">
-        <v>1.018373891140072</v>
+        <v>0.9807209403284943</v>
       </c>
       <c r="V21" t="n">
-        <v>0.9380567283075769</v>
+        <v>1.013929841949952</v>
       </c>
       <c r="W21" t="n">
-        <v>1.008609642550274</v>
+        <v>1.044232309049444</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>44425</v>
+        <v>44445</v>
       </c>
       <c r="B22" t="n">
-        <v>1.021842449465955</v>
+        <v>0.9991658789082624</v>
       </c>
       <c r="C22" t="n">
-        <v>1.035401190187927</v>
+        <v>1.021122828881062</v>
       </c>
       <c r="D22" t="n">
-        <v>0.9878135292927473</v>
+        <v>1.03742285878123</v>
       </c>
       <c r="E22" t="n">
-        <v>1.008225694954018</v>
+        <v>1.014421793577925</v>
       </c>
       <c r="F22" t="n">
-        <v>0.9853008476889036</v>
+        <v>1.01649681979775</v>
       </c>
       <c r="G22" t="n">
-        <v>1.016124543972326</v>
+        <v>0.9996618261876066</v>
       </c>
       <c r="H22" t="n">
-        <v>0.9593783298625596</v>
+        <v>1.029856914023133</v>
       </c>
       <c r="I22" t="n">
-        <v>1.021592031531882</v>
+        <v>1.005309204134837</v>
       </c>
       <c r="J22" t="n">
-        <v>1.021362353530288</v>
+        <v>1.033992787356695</v>
       </c>
       <c r="K22" t="n">
-        <v>1.028528321464107</v>
+        <v>1.002636538549249</v>
       </c>
       <c r="L22" t="n">
-        <v>0.9240682296442528</v>
+        <v>1.015368283949756</v>
       </c>
       <c r="M22" t="n">
-        <v>0.9379014672697755</v>
+        <v>1.052713172380314</v>
       </c>
       <c r="N22" t="n">
-        <v>0.9905671786846224</v>
+        <v>1.029179939274284</v>
       </c>
       <c r="O22" t="n">
-        <v>0.9373236461649109</v>
+        <v>0.9843482136241054</v>
       </c>
       <c r="P22" t="n">
-        <v>0.9445813034966376</v>
+        <v>1.173231730865591</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.9378835758944903</v>
+        <v>1.017269824800037</v>
       </c>
       <c r="R22" t="n">
-        <v>1.040979494524975</v>
+        <v>0.9193879333339653</v>
       </c>
       <c r="S22" t="n">
-        <v>0.7195583788754435</v>
+        <v>1.054622989287073</v>
       </c>
       <c r="T22" t="n">
-        <v>1.132880381344162</v>
+        <v>1.125321733033778</v>
       </c>
       <c r="U22" t="n">
-        <v>1.017455174679663</v>
+        <v>0.9815194766266907</v>
       </c>
       <c r="V22" t="n">
-        <v>0.9315789500779157</v>
+        <v>1.009629378244802</v>
       </c>
       <c r="W22" t="n">
-        <v>0.9969794551673065</v>
+        <v>1.045178062518132</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>44426</v>
+        <v>44446</v>
       </c>
       <c r="B23" t="n">
-        <v>1.02016331394248</v>
+        <v>0.9939108753017476</v>
       </c>
       <c r="C23" t="n">
-        <v>1.04164590855083</v>
+        <v>1.014768272239304</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9790334782721444</v>
+        <v>1.03766607236428</v>
       </c>
       <c r="E23" t="n">
-        <v>0.9973888105668562</v>
+        <v>1.013271006963828</v>
       </c>
       <c r="F23" t="n">
-        <v>0.9769783109111909</v>
+        <v>1.014054837015655</v>
       </c>
       <c r="G23" t="n">
-        <v>1.018933830873026</v>
+        <v>0.9940756163752351</v>
       </c>
       <c r="H23" t="n">
-        <v>0.9599168366678994</v>
+        <v>1.032089687972922</v>
       </c>
       <c r="I23" t="n">
-        <v>1.021914287203565</v>
+        <v>0.9996877078902843</v>
       </c>
       <c r="J23" t="n">
-        <v>1.027431106050847</v>
+        <v>1.028870264151415</v>
       </c>
       <c r="K23" t="n">
-        <v>1.029735853087227</v>
+        <v>0.9975098582081754</v>
       </c>
       <c r="L23" t="n">
-        <v>0.9084106861846114</v>
+        <v>1.010839716339584</v>
       </c>
       <c r="M23" t="n">
-        <v>0.9319057761622268</v>
+        <v>1.046976754831713</v>
       </c>
       <c r="N23" t="n">
-        <v>0.9913384463916436</v>
+        <v>1.022372674822858</v>
       </c>
       <c r="O23" t="n">
-        <v>0.9393390087399009</v>
+        <v>0.9757886479475567</v>
       </c>
       <c r="P23" t="n">
-        <v>0.9482758519441744</v>
+        <v>1.161372360385168</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.9263530025895529</v>
+        <v>1.016190447126116</v>
       </c>
       <c r="R23" t="n">
-        <v>1.040979494524975</v>
+        <v>0.9133932798679931</v>
       </c>
       <c r="S23" t="n">
-        <v>0.7381703470031544</v>
+        <v>1.035171875136266</v>
       </c>
       <c r="T23" t="n">
-        <v>1.133635314126574</v>
+        <v>1.133266240417669</v>
       </c>
       <c r="U23" t="n">
-        <v>1.016077187602672</v>
+        <v>0.9767282588375127</v>
       </c>
       <c r="V23" t="n">
-        <v>0.9207827903095362</v>
+        <v>1.005328914539652</v>
       </c>
       <c r="W23" t="n">
-        <v>0.9835772470051153</v>
+        <v>1.046041840296781</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>44427</v>
+        <v>44447</v>
       </c>
       <c r="B24" t="n">
-        <v>1.004453839753622</v>
+        <v>0.986417701070496</v>
       </c>
       <c r="C24" t="n">
-        <v>1.031616804655326</v>
+        <v>1.004299510082033</v>
       </c>
       <c r="D24" t="n">
-        <v>0.9801037683081726</v>
+        <v>1.031747545619025</v>
       </c>
       <c r="E24" t="n">
-        <v>0.9986422213382865</v>
+        <v>1.011934941515667</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9650487706732034</v>
+        <v>1.002522163719029</v>
       </c>
       <c r="G24" t="n">
-        <v>1.006159789691134</v>
+        <v>0.9794679660122757</v>
       </c>
       <c r="H24" t="n">
-        <v>0.944145180082348</v>
+        <v>1.016356413739912</v>
       </c>
       <c r="I24" t="n">
-        <v>1.00279301908324</v>
+        <v>0.9895898394189525</v>
       </c>
       <c r="J24" t="n">
-        <v>1.022887662910292</v>
+        <v>1.023448726981424</v>
       </c>
       <c r="K24" t="n">
-        <v>1.01464152785967</v>
+        <v>0.9866705612674276</v>
       </c>
       <c r="L24" t="n">
-        <v>0.8847166425673501</v>
+        <v>1.024569979596139</v>
       </c>
       <c r="M24" t="n">
-        <v>0.9211991382215098</v>
+        <v>1.03116279424623</v>
       </c>
       <c r="N24" t="n">
-        <v>0.9884314370165769</v>
+        <v>1.01981224172773</v>
       </c>
       <c r="O24" t="n">
-        <v>0.9153566938059605</v>
+        <v>0.9600670260795585</v>
       </c>
       <c r="P24" t="n">
-        <v>0.9433497481982661</v>
+        <v>1.249047022445761</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.929514582792232</v>
+        <v>0.9952380952380955</v>
       </c>
       <c r="R24" t="n">
-        <v>1.022488698173092</v>
+        <v>0.9148130947206701</v>
       </c>
       <c r="S24" t="n">
-        <v>0.7164038047429514</v>
+        <v>0.994204648417553</v>
       </c>
       <c r="T24" t="n">
-        <v>1.089090247819098</v>
+        <v>1.133266240417669</v>
       </c>
       <c r="U24" t="n">
-        <v>1.011713328222538</v>
+        <v>0.9719369540144056</v>
       </c>
       <c r="V24" t="n">
-        <v>0.8967611108851694</v>
+        <v>1.01809004290692</v>
       </c>
       <c r="W24" t="n">
-        <v>0.9824043968503181</v>
+        <v>1.038134447393463</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>44428</v>
+        <v>44448</v>
       </c>
       <c r="B25" t="n">
-        <v>1.008580426297679</v>
+        <v>0.9765055892493953</v>
       </c>
       <c r="C25" t="n">
-        <v>1.037909575727015</v>
+        <v>1.002236074234342</v>
       </c>
       <c r="D25" t="n">
-        <v>0.991755061087687</v>
+        <v>1.029156497065289</v>
       </c>
       <c r="E25" t="n">
-        <v>1.006772734547189</v>
+        <v>1.007274365188304</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9809699244016445</v>
+        <v>1.002254748871021</v>
       </c>
       <c r="G25" t="n">
-        <v>1.008854900231861</v>
+        <v>0.9802755022821678</v>
       </c>
       <c r="H25" t="n">
-        <v>0.9430681664716684</v>
+        <v>1.014720791381469</v>
       </c>
       <c r="I25" t="n">
-        <v>1.006982506729505</v>
+        <v>0.9801166345902748</v>
       </c>
       <c r="J25" t="n">
-        <v>1.023228458285696</v>
+        <v>1.019663842218985</v>
       </c>
       <c r="K25" t="n">
-        <v>1.018415127160414</v>
+        <v>0.9860846250088272</v>
       </c>
       <c r="L25" t="n">
-        <v>0.8847166425673501</v>
+        <v>1.007804608996576</v>
       </c>
       <c r="M25" t="n">
-        <v>0.914346896474264</v>
+        <v>1.035813974779706</v>
       </c>
       <c r="N25" t="n">
-        <v>0.9889653498024935</v>
+        <v>1.024323370254011</v>
       </c>
       <c r="O25" t="n">
-        <v>0.9358122203314454</v>
+        <v>0.9567130832796245</v>
       </c>
       <c r="P25" t="n">
-        <v>0.9482758519441743</v>
+        <v>1.27827199058492</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.9220755329916682</v>
+        <v>0.9830476306733634</v>
       </c>
       <c r="R25" t="n">
-        <v>0.9975011922120315</v>
+        <v>0.9115002836650884</v>
       </c>
       <c r="S25" t="n">
-        <v>0.7487381896009955</v>
+        <v>1.000399704655217</v>
       </c>
       <c r="T25" t="n">
-        <v>1.106077790679362</v>
+        <v>1.138972792026542</v>
       </c>
       <c r="U25" t="n">
-        <v>1.017914532909867</v>
+        <v>0.9657768665905646</v>
       </c>
       <c r="V25" t="n">
-        <v>0.8796221544854612</v>
+        <v>1.001963250518042</v>
       </c>
       <c r="W25" t="n">
-        <v>0.9992485627933597</v>
+        <v>1.029226048831849</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>44430</v>
+        <v>44449</v>
       </c>
       <c r="B26" t="n">
-        <v>1.01008165697124</v>
+        <v>0.9772006901591765</v>
       </c>
       <c r="C26" t="n">
-        <v>1.037682328236531</v>
+        <v>0.9994440863004415</v>
       </c>
       <c r="D26" t="n">
-        <v>0.999438231015466</v>
+        <v>1.020196086831863</v>
       </c>
       <c r="E26" t="n">
-        <v>1.011063494414049</v>
+        <v>0.9994956095702833</v>
       </c>
       <c r="F26" t="n">
-        <v>0.9901795170906731</v>
+        <v>0.9926383673289988</v>
       </c>
       <c r="G26" t="n">
-        <v>1.010282852611594</v>
+        <v>0.9794384317166472</v>
       </c>
       <c r="H26" t="n">
-        <v>0.950223103726328</v>
+        <v>1.01363034478326</v>
       </c>
       <c r="I26" t="n">
-        <v>1.006982506729505</v>
+        <v>0.9944826275997605</v>
       </c>
       <c r="J26" t="n">
-        <v>1.025175626980298</v>
+        <v>1.01910519614807</v>
       </c>
       <c r="K26" t="n">
-        <v>1.021735857117851</v>
+        <v>0.9837410196659881</v>
       </c>
       <c r="L26" t="n">
-        <v>0.9081336092333331</v>
+        <v>1.030640194282155</v>
       </c>
       <c r="M26" t="n">
-        <v>0.9256959065521714</v>
+        <v>1.022790687028752</v>
       </c>
       <c r="N26" t="n">
-        <v>0.9949869409531199</v>
+        <v>1.019141669825427</v>
       </c>
       <c r="O26" t="n">
-        <v>0.9447299787008892</v>
+        <v>0.9375326854092338</v>
       </c>
       <c r="P26" t="n">
-        <v>0.9599753630216535</v>
+        <v>1.255400286926312</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.9255161032793271</v>
+        <v>0.982666669573103</v>
       </c>
       <c r="R26" t="n">
-        <v>0.9975011922120315</v>
+        <v>0.9214387168318334</v>
       </c>
       <c r="S26" t="n">
-        <v>0.7677444794952679</v>
+        <v>1.015587566757965</v>
       </c>
       <c r="T26" t="n">
-        <v>1.113061581340522</v>
+        <v>1.147700573687454</v>
       </c>
       <c r="U26" t="n">
-        <v>1.026871799364801</v>
+        <v>0.966461301407896</v>
       </c>
       <c r="V26" t="n">
-        <v>0.9037112217482022</v>
+        <v>1.022577487946605</v>
       </c>
       <c r="W26" t="n">
-        <v>1.011679205039534</v>
+        <v>1.020482487919508</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>44431</v>
+        <v>44451</v>
       </c>
       <c r="B27" t="n">
-        <v>1.011582887644802</v>
+        <v>0.9799254653612344</v>
       </c>
       <c r="C27" t="n">
-        <v>1.037455080746048</v>
+        <v>1.000330513271443</v>
       </c>
       <c r="D27" t="n">
-        <v>1.007121400943245</v>
+        <v>1.019861651677284</v>
       </c>
       <c r="E27" t="n">
-        <v>1.01535425428091</v>
+        <v>1.000633279260228</v>
       </c>
       <c r="F27" t="n">
-        <v>0.9993891097797016</v>
+        <v>0.9955861318964445</v>
       </c>
       <c r="G27" t="n">
-        <v>1.011710804991327</v>
+        <v>0.9823124802006863</v>
       </c>
       <c r="H27" t="n">
-        <v>0.9573780409809876</v>
+        <v>1.01363034478326</v>
       </c>
       <c r="I27" t="n">
-        <v>1.006982506729505</v>
+        <v>0.9944826275997605</v>
       </c>
       <c r="J27" t="n">
-        <v>1.0271227956749</v>
+        <v>1.015402965261839</v>
       </c>
       <c r="K27" t="n">
-        <v>1.025056587075288</v>
+        <v>0.985059323863503</v>
       </c>
       <c r="L27" t="n">
-        <v>0.9315505758993161</v>
+        <v>1.030640194282155</v>
       </c>
       <c r="M27" t="n">
-        <v>0.9370449166300787</v>
+        <v>1.022790687028752</v>
       </c>
       <c r="N27" t="n">
-        <v>1.001008532103747</v>
+        <v>1.02084860971906</v>
       </c>
       <c r="O27" t="n">
-        <v>0.9536477370703329</v>
+        <v>0.9395241164344242</v>
       </c>
       <c r="P27" t="n">
-        <v>0.9716748740991328</v>
+        <v>1.255400286926312</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.928956673566986</v>
+        <v>0.9810476030622213</v>
       </c>
       <c r="R27" t="n">
-        <v>0.9975011922120315</v>
+        <v>0.9185991773938107</v>
       </c>
       <c r="S27" t="n">
-        <v>0.7867507693895404</v>
+        <v>1.015587566757965</v>
       </c>
       <c r="T27" t="n">
-        <v>1.120045372001682</v>
+        <v>1.147700573687454</v>
       </c>
       <c r="U27" t="n">
-        <v>1.035829065819735</v>
+        <v>0.9623545184360494</v>
       </c>
       <c r="V27" t="n">
-        <v>0.9278002890109431</v>
+        <v>1.022577487946605</v>
       </c>
       <c r="W27" t="n">
-        <v>1.023991206602278</v>
+        <v>1.017748927905479</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>44432</v>
+        <v>44452</v>
       </c>
       <c r="B28" t="n">
-        <v>1.013973434126396</v>
+        <v>0.9826502405632921</v>
       </c>
       <c r="C28" t="n">
-        <v>1.0438134015164</v>
+        <v>1.001216940242444</v>
       </c>
       <c r="D28" t="n">
-        <v>1.012321203116314</v>
+        <v>1.019527216522705</v>
       </c>
       <c r="E28" t="n">
-        <v>1.016872956497737</v>
+        <v>1.001770948950172</v>
       </c>
       <c r="F28" t="n">
-        <v>1.009621438103419</v>
+        <v>0.9985338964638901</v>
       </c>
       <c r="G28" t="n">
-        <v>1.015097019055922</v>
+        <v>0.9851865286847252</v>
       </c>
       <c r="H28" t="n">
-        <v>0.9796122488040433</v>
+        <v>1.01363034478326</v>
       </c>
       <c r="I28" t="n">
-        <v>1.006982506729505</v>
+        <v>0.9944826275997605</v>
       </c>
       <c r="J28" t="n">
-        <v>1.032323465816669</v>
+        <v>1.011700734375608</v>
       </c>
       <c r="K28" t="n">
-        <v>1.025056587075288</v>
+        <v>0.9863776280610179</v>
       </c>
       <c r="L28" t="n">
-        <v>0.9578772205534647</v>
+        <v>1.030640194282155</v>
       </c>
       <c r="M28" t="n">
-        <v>0.9456102596567183</v>
+        <v>1.022790687028752</v>
       </c>
       <c r="N28" t="n">
-        <v>1.000533912785917</v>
+        <v>1.022555549612693</v>
       </c>
       <c r="O28" t="n">
-        <v>0.9507255189952636</v>
+        <v>0.9415155474596146</v>
       </c>
       <c r="P28" t="n">
-        <v>0.959359614734362</v>
+        <v>1.255400286926312</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.9600148501473842</v>
+        <v>0.9794285365513395</v>
       </c>
       <c r="R28" t="n">
-        <v>1.012993514538124</v>
+        <v>0.915759637955788</v>
       </c>
       <c r="S28" t="n">
-        <v>0.7572555301317279</v>
+        <v>1.015587566757965</v>
       </c>
       <c r="T28" t="n">
-        <v>1.124952838301877</v>
+        <v>1.147700573687454</v>
       </c>
       <c r="U28" t="n">
-        <v>1.040192925199868</v>
+        <v>0.9582477354642027</v>
       </c>
       <c r="V28" t="n">
-        <v>0.9588394671367169</v>
+        <v>1.022577487946605</v>
       </c>
       <c r="W28" t="n">
-        <v>1.030035432047099</v>
+        <v>1.014909859235674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>